<commit_message>
added and renamed attributes
</commit_message>
<xml_diff>
--- a/dist/ernithaca.xlsx
+++ b/dist/ernithaca.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="101">
   <si>
     <t>ernstats</t>
   </si>
@@ -25,7 +25,7 @@
     <t>ERN Ithaca Stats</t>
   </si>
   <si>
-    <t>Descriptives on enrolled patients and data providers (v1.1.1, 2022-10-10)</t>
+    <t>Descriptives on enrolled patients and data providers (v1.2.0, 2022-12-01)</t>
   </si>
   <si>
     <t>dataproviders</t>
@@ -52,159 +52,183 @@
     <t>ernstats_stats</t>
   </si>
   <si>
+    <t>iri</t>
+  </si>
+  <si>
+    <t>codesystem</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>centerType</t>
+  </si>
+  <si>
+    <t>centerRepresentative</t>
+  </si>
+  <si>
+    <t>hasSubmittedData</t>
+  </si>
+  <si>
+    <t>additionalInformation</t>
+  </si>
+  <si>
+    <t>displayName</t>
+  </si>
+  <si>
+    <t>officialName</t>
+  </si>
+  <si>
+    <t>centerProjectUrl</t>
+  </si>
+  <si>
+    <t>centerLocation</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>valueOrder</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>compound</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>A unique symbol that establishes identity of the resource.</t>
+  </si>
+  <si>
+    <t>A systematized collection of concepts that define corresponding codes.</t>
+  </si>
+  <si>
+    <t>A symbol or combination of symbols which is assigned to the members of a collection.</t>
+  </si>
+  <si>
+    <t>Original institution name as defined by the project</t>
+  </si>
+  <si>
+    <t>An indication that a file has been submitted to a data repository.</t>
+  </si>
+  <si>
+    <t>The standardized text associated with a code in a particular code system.</t>
+  </si>
+  <si>
+    <t>An established society, corporation, foundation or other organization founded and united for a specific purpose, e.g. for health-related research; also used to refer to a building or buildings occupied or used by such organization.</t>
+  </si>
+  <si>
+    <t>A large and densely populated urban area; a city specified in an address.</t>
+  </si>
+  <si>
+    <t>A collective generic term that refers here to a wide variety of dependencies, areas of special sovereignty, uninhabited islands, and other entities in addition to the traditional countries or independent states.</t>
+  </si>
+  <si>
+    <t>The angular distance north or south between an imaginary line around a heavenly body parallel to its equator and the equator itself.</t>
+  </si>
+  <si>
+    <t>An imaginary great circle on the surface of a heavenly body passing through the poles at right angles to the equator.</t>
+  </si>
+  <si>
+    <t>title to be rendered into the app (e.g., section heading, component title, table heading, etc)</t>
+  </si>
+  <si>
+    <t>string that describes the value</t>
+  </si>
+  <si>
+    <t>raw data value</t>
+  </si>
+  <si>
+    <t>integer specifying the order of a value in an array (ideal for tables, charts)</t>
+  </si>
+  <si>
+    <t>name of the component that the current will be used in</t>
+  </si>
+  <si>
+    <t>additional information about this record</t>
+  </si>
+  <si>
+    <t>NCIT_C165071</t>
+  </si>
+  <si>
+    <t>NCIT_C70895</t>
+  </si>
+  <si>
+    <t>NCIT_C25162</t>
+  </si>
+  <si>
+    <t>NCIT_C51875</t>
+  </si>
+  <si>
+    <t>NCIT_C172872</t>
+  </si>
+  <si>
+    <t>NCIT_C70896</t>
+  </si>
+  <si>
+    <t>NCIT_C25341</t>
+  </si>
+  <si>
+    <t>NCIT_C25160</t>
+  </si>
+  <si>
+    <t>NCIT_C25464</t>
+  </si>
+  <si>
+    <t>NCIT_C68642</t>
+  </si>
+  <si>
+    <t>NCIT_C68643</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
-    <t>displayName</t>
-  </si>
-  <si>
-    <t>hasSubmittedData</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>codesystem</t>
-  </si>
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>iri</t>
-  </si>
-  <si>
-    <t>projectName</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>label</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>valueOrder</t>
-  </si>
-  <si>
-    <t>component</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>An established society, corporation, foundation or other organization founded and united for a specific purpose, e.g. for health-related research; also used to refer to a building or buildings occupied or used by such organization.</t>
-  </si>
-  <si>
-    <t>The standardized text associated with a code in a particular code system.</t>
-  </si>
-  <si>
-    <t>An indication that a file has been submitted to a data repository.</t>
-  </si>
-  <si>
-    <t>A large and densely populated urban area; a city specified in an address.</t>
-  </si>
-  <si>
-    <t>A collective generic term that refers here to a wide variety of dependencies, areas of special sovereignty, uninhabited islands, and other entities in addition to the traditional countries or independent states.</t>
-  </si>
-  <si>
-    <t>An imaginary great circle on the surface of a heavenly body passing through the poles at right angles to the equator.</t>
-  </si>
-  <si>
-    <t>The angular distance north or south between an imaginary line around a heavenly body parallel to its equator and the equator itself.</t>
-  </si>
-  <si>
-    <t>A systematized collection of concepts that define corresponding codes.</t>
-  </si>
-  <si>
-    <t>A symbol or combination of symbols which is assigned to the members of a collection.</t>
-  </si>
-  <si>
-    <t>A unique symbol that establishes identity of the resource.</t>
-  </si>
-  <si>
-    <t>Original institution name as defined by the GENTURIS project (prior to cleaning)</t>
-  </si>
-  <si>
-    <t>title to be rendered into the app (e.g., section heading, component title, table heading, etc)</t>
-  </si>
-  <si>
-    <t>string that describes the value</t>
-  </si>
-  <si>
-    <t>raw data value</t>
-  </si>
-  <si>
-    <t>integer specifying the order of a value in an array (ideal for tables, charts)</t>
-  </si>
-  <si>
-    <t>name of the component that the current will be used in</t>
-  </si>
-  <si>
-    <t>additional information about this record</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
-    <t>hyperlink</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>NCIT_C41206</t>
-  </si>
-  <si>
-    <t>NCIT_C70896</t>
-  </si>
-  <si>
-    <t>NCIT_C172872</t>
-  </si>
-  <si>
-    <t>NCIT_C25160</t>
-  </si>
-  <si>
-    <t>NCIT_C25464</t>
-  </si>
-  <si>
-    <t>NCIT_C68643</t>
-  </si>
-  <si>
-    <t>NCIT_C68642</t>
-  </si>
-  <si>
-    <t>NCIT_C70895</t>
-  </si>
-  <si>
-    <t>NCIT_C25162</t>
-  </si>
-  <si>
-    <t>NCIT_C165071</t>
-  </si>
-  <si>
     <t>package</t>
   </si>
   <si>
@@ -214,6 +238,9 @@
     <t>dataType</t>
   </si>
   <si>
+    <t>tags</t>
+  </si>
+  <si>
     <t>idAttribute</t>
   </si>
   <si>
@@ -226,46 +253,49 @@
     <t>nillable</t>
   </si>
   <si>
+    <t>visible</t>
+  </si>
+  <si>
+    <t>partOfAttribute</t>
+  </si>
+  <si>
     <t>readOnly</t>
   </si>
   <si>
-    <t>tags</t>
-  </si>
-  <si>
-    <t>visible</t>
-  </si>
-  <si>
     <t>defaultValue</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70895</t>
   </si>
   <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25341</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C172872</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
+  </si>
+  <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25162</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C172872</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C51875</t>
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/NCIT_C70896</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C41206</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C165071</t>
   </si>
   <si>
     <t>NCIT</t>
@@ -657,13 +687,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -692,16 +722,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -739,51 +769,54 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+        <v>80</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -791,13 +824,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -806,71 +839,62 @@
         <v>1</v>
       </c>
       <c r="H2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
       <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
       <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -878,25 +902,22 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>44</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -904,25 +925,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>35</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -930,25 +945,22 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -956,25 +968,25 @@
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -982,22 +994,19 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>37</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1005,22 +1014,28 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1028,25 +1043,25 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>47</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1054,166 +1069,181 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>34</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="b">
         <v>0</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="K13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>66</v>
       </c>
       <c r="F15" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="K17" t="b">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>10</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="K18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -1221,18 +1251,142 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" t="b">
+        <v>52</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1243,7 +1397,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1251,202 +1405,202 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1457,16 +1611,36 @@
         <v>61</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1491,6 +1665,8 @@
     <hyperlink ref="F10" r:id="rId18" location="isAssociatedWith"/>
     <hyperlink ref="C11" r:id="rId19"/>
     <hyperlink ref="F11" r:id="rId20" location="isAssociatedWith"/>
+    <hyperlink ref="C12" r:id="rId21"/>
+    <hyperlink ref="F12" r:id="rId22" location="isAssociatedWith"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>